<commit_message>
Fix all Country names for Tableau fuckerrr
</commit_message>
<xml_diff>
--- a/data/main.xlsx
+++ b/data/main.xlsx
@@ -43,13 +43,13 @@
     <t>Albania</t>
   </si>
   <si>
-    <t>Andorra, Principality of</t>
+    <t>Andorra</t>
   </si>
   <si>
     <t>Austria</t>
   </si>
   <si>
-    <t>Belarus, Rep. of</t>
+    <t>Belarus</t>
   </si>
   <si>
     <t>Belgium</t>
@@ -61,16 +61,16 @@
     <t>Bulgaria</t>
   </si>
   <si>
-    <t>Croatia, Rep. of</t>
+    <t>Croatia</t>
   </si>
   <si>
-    <t>Czech Rep.</t>
+    <t>Czech Republic</t>
   </si>
   <si>
     <t>Denmark</t>
   </si>
   <si>
-    <t>Estonia, Rep. of</t>
+    <t>Estonia</t>
   </si>
   <si>
     <t>Finland</t>
@@ -91,7 +91,7 @@
     <t>Iceland</t>
   </si>
   <si>
-    <t>Ireland</t>
+    <t>Republic of Ireland</t>
   </si>
   <si>
     <t>Italy</t>
@@ -112,22 +112,22 @@
     <t>Malta</t>
   </si>
   <si>
-    <t>Moldova, Rep. of</t>
+    <t>Moldova</t>
   </si>
   <si>
     <t>Montenegro</t>
   </si>
   <si>
-    <t>Netherlands, The</t>
+    <t>Kingdom of the Netherlands</t>
   </si>
   <si>
-    <t xml:space="preserve">North Macedonia, Republic of </t>
+    <t>Macedonia</t>
   </si>
   <si>
     <t>Norway</t>
   </si>
   <si>
-    <t>Poland, Rep. of</t>
+    <t>Poland</t>
   </si>
   <si>
     <t>Portugal</t>
@@ -136,13 +136,13 @@
     <t>Romania</t>
   </si>
   <si>
-    <t>Serbia, Rep. of</t>
+    <t>Serbia</t>
   </si>
   <si>
-    <t>Slovak Rep.</t>
+    <t>Slovakia</t>
   </si>
   <si>
-    <t>Slovenia, Rep. of</t>
+    <t>Slovenia</t>
   </si>
   <si>
     <t>Spain</t>

</xml_diff>

<commit_message>
Added total and average for each year
</commit_message>
<xml_diff>
--- a/data/main.xlsx
+++ b/data/main.xlsx
@@ -9,13 +9,14 @@
   <sheets>
     <sheet name="main" sheetId="1" r:id="rId1"/>
     <sheet name="average" sheetId="2" r:id="rId2"/>
+    <sheet name="total" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1215" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1221" uniqueCount="129">
   <si>
     <t>country</t>
   </si>
@@ -13062,4 +13063,267 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:G11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="B1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" s="1">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>2012</v>
+      </c>
+      <c r="C2">
+        <v>56.51300000000001</v>
+      </c>
+      <c r="D2">
+        <v>4284036292</v>
+      </c>
+      <c r="E2">
+        <v>18899062187231.49</v>
+      </c>
+      <c r="F2">
+        <v>0.6503946</v>
+      </c>
+      <c r="G2">
+        <v>591702029</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>2013</v>
+      </c>
+      <c r="C3">
+        <v>39.975</v>
+      </c>
+      <c r="D3">
+        <v>4187930277</v>
+      </c>
+      <c r="E3">
+        <v>19710492567527.39</v>
+      </c>
+      <c r="F3">
+        <v>4.1503489</v>
+      </c>
+      <c r="G3">
+        <v>593142931</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" s="1">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>2014</v>
+      </c>
+      <c r="C4">
+        <v>79.292</v>
+      </c>
+      <c r="D4">
+        <v>3958391776</v>
+      </c>
+      <c r="E4">
+        <v>20293345323920.78</v>
+      </c>
+      <c r="F4">
+        <v>16.3897677</v>
+      </c>
+      <c r="G4">
+        <v>594565062</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" s="1">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <v>2015</v>
+      </c>
+      <c r="C5">
+        <v>68.438</v>
+      </c>
+      <c r="D5">
+        <v>3960306862</v>
+      </c>
+      <c r="E5">
+        <v>17839800156187.61</v>
+      </c>
+      <c r="F5">
+        <v>27.0352689</v>
+      </c>
+      <c r="G5">
+        <v>595963744</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6" s="1">
+        <v>4</v>
+      </c>
+      <c r="B6">
+        <v>2016</v>
+      </c>
+      <c r="C6">
+        <v>72.72999999999998</v>
+      </c>
+      <c r="D6">
+        <v>3957305821.9</v>
+      </c>
+      <c r="E6">
+        <v>17923128827861.67</v>
+      </c>
+      <c r="F6">
+        <v>31.1519053</v>
+      </c>
+      <c r="G6">
+        <v>597279081</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" s="1">
+        <v>5</v>
+      </c>
+      <c r="B7">
+        <v>2017</v>
+      </c>
+      <c r="C7">
+        <v>60.252</v>
+      </c>
+      <c r="D7">
+        <v>3960139110</v>
+      </c>
+      <c r="E7">
+        <v>18847422473370.02</v>
+      </c>
+      <c r="F7">
+        <v>65.9753953</v>
+      </c>
+      <c r="G7">
+        <v>598240534</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" s="1">
+        <v>6</v>
+      </c>
+      <c r="B8">
+        <v>2018</v>
+      </c>
+      <c r="C8">
+        <v>81.67700000000002</v>
+      </c>
+      <c r="D8">
+        <v>3887174521</v>
+      </c>
+      <c r="E8">
+        <v>20369250013115.85</v>
+      </c>
+      <c r="F8">
+        <v>82.98431329999998</v>
+      </c>
+      <c r="G8">
+        <v>599120957</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" s="1">
+        <v>7</v>
+      </c>
+      <c r="B9">
+        <v>2019</v>
+      </c>
+      <c r="C9">
+        <v>79.45500000000001</v>
+      </c>
+      <c r="D9">
+        <v>3717680253</v>
+      </c>
+      <c r="E9">
+        <v>20051444797403.53</v>
+      </c>
+      <c r="F9">
+        <v>151.7125718</v>
+      </c>
+      <c r="G9">
+        <v>599504550</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10" s="1">
+        <v>8</v>
+      </c>
+      <c r="B10">
+        <v>2020</v>
+      </c>
+      <c r="C10">
+        <v>92.11499999999999</v>
+      </c>
+      <c r="D10">
+        <v>3370241592</v>
+      </c>
+      <c r="E10">
+        <v>19506692418091.7</v>
+      </c>
+      <c r="F10">
+        <v>168.0720224</v>
+      </c>
+      <c r="G10">
+        <v>599695156</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="A11" s="1">
+        <v>9</v>
+      </c>
+      <c r="B11">
+        <v>2021</v>
+      </c>
+      <c r="C11">
+        <v>59.56900000000001</v>
+      </c>
+      <c r="D11">
+        <v>3536737297</v>
+      </c>
+      <c r="E11">
+        <v>21977425645774.62</v>
+      </c>
+      <c r="F11">
+        <v>318.1558474999999</v>
+      </c>
+      <c r="G11">
+        <v>598984930</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Python og Dæsh clean
</commit_message>
<xml_diff>
--- a/data/main.xlsx
+++ b/data/main.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3111" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3113" uniqueCount="112">
   <si>
     <t>ISO2</t>
   </si>
@@ -349,6 +349,9 @@
   </si>
   <si>
     <t>ev sales share change</t>
+  </si>
+  <si>
+    <t>Emission change since 1990</t>
   </si>
 </sst>
 </file>
@@ -40430,13 +40433,13 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J33"/>
+  <dimension ref="A1:L33"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:12">
       <c r="B1" s="1" t="s">
         <v>2</v>
       </c>
@@ -40464,8 +40467,14 @@
       <c r="J1" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="2" spans="1:10">
+      <c r="K1" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12">
       <c r="A2" s="1">
         <v>29</v>
       </c>
@@ -40493,8 +40502,14 @@
       <c r="J2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:10">
+      <c r="K2">
+        <v>0</v>
+      </c>
+      <c r="L2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12">
       <c r="A3" s="1">
         <v>30</v>
       </c>
@@ -40525,8 +40540,14 @@
       <c r="J3">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:10">
+      <c r="K3">
+        <v>-0.01202191061694069</v>
+      </c>
+      <c r="L3">
+        <v>-0.01202191061694069</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12">
       <c r="A4" s="1">
         <v>31</v>
       </c>
@@ -40557,8 +40578,14 @@
       <c r="J4">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:10">
+      <c r="K4">
+        <v>-0.04351763000623127</v>
+      </c>
+      <c r="L4">
+        <v>-0.04351763000623127</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12">
       <c r="A5" s="1">
         <v>32</v>
       </c>
@@ -40589,8 +40616,14 @@
       <c r="J5">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:10">
+      <c r="K5">
+        <v>-0.061601803895558</v>
+      </c>
+      <c r="L5">
+        <v>-0.061601803895558</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12">
       <c r="A6" s="1">
         <v>33</v>
       </c>
@@ -40621,8 +40654,14 @@
       <c r="J6">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:10">
+      <c r="K6">
+        <v>-0.06669553566309869</v>
+      </c>
+      <c r="L6">
+        <v>-0.06669553566309869</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12">
       <c r="A7" s="1">
         <v>34</v>
       </c>
@@ -40653,8 +40692,14 @@
       <c r="J7">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:10">
+      <c r="K7">
+        <v>-0.05751285579002759</v>
+      </c>
+      <c r="L7">
+        <v>-0.05751285579002759</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12">
       <c r="A8" s="1">
         <v>35</v>
       </c>
@@ -40682,8 +40727,14 @@
       <c r="J8">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:10">
+      <c r="K8">
+        <v>-0.03369104134656577</v>
+      </c>
+      <c r="L8">
+        <v>-0.03369104134656577</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12">
       <c r="A9" s="1">
         <v>36</v>
       </c>
@@ -40711,8 +40762,14 @@
       <c r="J9">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:10">
+      <c r="K9">
+        <v>-0.05364898870356756</v>
+      </c>
+      <c r="L9">
+        <v>-0.05364898870356756</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12">
       <c r="A10" s="1">
         <v>37</v>
       </c>
@@ -40740,8 +40797,14 @@
       <c r="J10">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:10">
+      <c r="K10">
+        <v>-0.05397081384077276</v>
+      </c>
+      <c r="L10">
+        <v>-0.05397081384077276</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12">
       <c r="A11" s="1">
         <v>38</v>
       </c>
@@ -40772,8 +40835,14 @@
       <c r="J11">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:10">
+      <c r="K11">
+        <v>-0.06743642905450249</v>
+      </c>
+      <c r="L11">
+        <v>-0.06743642905450249</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12">
       <c r="A12" s="1">
         <v>39</v>
       </c>
@@ -40804,8 +40873,14 @@
       <c r="J12">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:10">
+      <c r="K12">
+        <v>-0.06347046317449073</v>
+      </c>
+      <c r="L12">
+        <v>-0.06347046317449073</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12">
       <c r="A13" s="1">
         <v>40</v>
       </c>
@@ -40836,8 +40911,14 @@
       <c r="J13">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:10">
+      <c r="K13">
+        <v>-0.04824994195643079</v>
+      </c>
+      <c r="L13">
+        <v>-0.04824994195643079</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12">
       <c r="A14" s="1">
         <v>41</v>
       </c>
@@ -40868,8 +40949,14 @@
       <c r="J14">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:10">
+      <c r="K14">
+        <v>-0.05235420932691991</v>
+      </c>
+      <c r="L14">
+        <v>-0.05235420932691991</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12">
       <c r="A15" s="1">
         <v>42</v>
       </c>
@@ -40900,8 +40987,14 @@
       <c r="J15">
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:10">
+      <c r="K15">
+        <v>-0.03101825529906309</v>
+      </c>
+      <c r="L15">
+        <v>-0.03101825529906309</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12">
       <c r="A16" s="1">
         <v>43</v>
       </c>
@@ -40932,8 +41025,14 @@
       <c r="J16">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:10">
+      <c r="K16">
+        <v>-0.02796066617184709</v>
+      </c>
+      <c r="L16">
+        <v>-0.02796066617184709</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12">
       <c r="A17" s="1">
         <v>44</v>
       </c>
@@ -40964,8 +41063,14 @@
       <c r="J17">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:10">
+      <c r="K17">
+        <v>-0.03309562249927574</v>
+      </c>
+      <c r="L17">
+        <v>-0.03309562249927574</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12">
       <c r="A18" s="1">
         <v>45</v>
       </c>
@@ -40993,8 +41098,14 @@
       <c r="J18">
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:10">
+      <c r="K18">
+        <v>-0.03141587660430183</v>
+      </c>
+      <c r="L18">
+        <v>-0.03141587660430183</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12">
       <c r="A19" s="1">
         <v>46</v>
       </c>
@@ -41022,8 +41133,14 @@
       <c r="J19">
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="1:10">
+      <c r="K19">
+        <v>-0.04093695694979146</v>
+      </c>
+      <c r="L19">
+        <v>-0.04093695694979146</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12">
       <c r="A20" s="1">
         <v>47</v>
       </c>
@@ -41054,8 +41171,14 @@
       <c r="J20">
         <v>0</v>
       </c>
-    </row>
-    <row r="21" spans="1:10">
+      <c r="K20">
+        <v>-0.06233409527205656</v>
+      </c>
+      <c r="L20">
+        <v>-0.06233409527205656</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12">
       <c r="A21" s="1">
         <v>48</v>
       </c>
@@ -41086,8 +41209,14 @@
       <c r="J21">
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="1:10">
+      <c r="K21">
+        <v>-0.138952652113448</v>
+      </c>
+      <c r="L21">
+        <v>-0.138952652113448</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12">
       <c r="A22" s="1">
         <v>49</v>
       </c>
@@ -41118,8 +41247,14 @@
       <c r="J22">
         <v>0.008092999918153503</v>
       </c>
-    </row>
-    <row r="23" spans="1:10">
+      <c r="K22">
+        <v>-0.1121153920739042</v>
+      </c>
+      <c r="L22">
+        <v>-0.1121153920739042</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12">
       <c r="A23" s="1">
         <v>50</v>
       </c>
@@ -41150,8 +41285,14 @@
       <c r="J23">
         <v>0.02506099969614297</v>
       </c>
-    </row>
-    <row r="24" spans="1:10">
+      <c r="K23">
+        <v>-0.1444294180427219</v>
+      </c>
+      <c r="L23">
+        <v>-0.1444294180427219</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12">
       <c r="A24" s="1">
         <v>51</v>
       </c>
@@ -41182,8 +41323,14 @@
       <c r="J24">
         <v>0.06409199887420983</v>
       </c>
-    </row>
-    <row r="25" spans="1:10">
+      <c r="K24">
+        <v>-0.1563513303875175</v>
+      </c>
+      <c r="L24">
+        <v>-0.1563513303875175</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12">
       <c r="A25" s="1">
         <v>52</v>
       </c>
@@ -41214,8 +41361,14 @@
       <c r="J25">
         <v>0.1541520023252815</v>
       </c>
-    </row>
-    <row r="26" spans="1:10">
+      <c r="K25">
+        <v>-0.1765019482381661</v>
+      </c>
+      <c r="L25">
+        <v>-0.1765019482381661</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12">
       <c r="A26" s="1">
         <v>53</v>
       </c>
@@ -41246,8 +41399,14 @@
       <c r="J26">
         <v>0.2629299997538329</v>
       </c>
-    </row>
-    <row r="27" spans="1:10">
+      <c r="K26">
+        <v>-0.2159172358664213</v>
+      </c>
+      <c r="L26">
+        <v>-0.2159172358664213</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12">
       <c r="A27" s="1">
         <v>54</v>
       </c>
@@ -41278,8 +41437,14 @@
       <c r="J27">
         <v>0.4715900035947562</v>
       </c>
-    </row>
-    <row r="28" spans="1:10">
+      <c r="K27">
+        <v>-0.2079325709182091</v>
+      </c>
+      <c r="L27">
+        <v>-0.2079325709182091</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12">
       <c r="A28" s="1">
         <v>55</v>
       </c>
@@ -41310,8 +41475,14 @@
       <c r="J28">
         <v>0.5466200009733438</v>
       </c>
-    </row>
-    <row r="29" spans="1:10">
+      <c r="K28">
+        <v>-0.2115464138571911</v>
+      </c>
+      <c r="L28">
+        <v>-0.2115464138571911</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12">
       <c r="A29" s="1">
         <v>56</v>
       </c>
@@ -41342,8 +41513,14 @@
       <c r="J29">
         <v>0.7537999989837407</v>
       </c>
-    </row>
-    <row r="30" spans="1:10">
+      <c r="K29">
+        <v>-0.209345677212742</v>
+      </c>
+      <c r="L29">
+        <v>-0.209345677212742</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12">
       <c r="A30" s="1">
         <v>57</v>
       </c>
@@ -41374,8 +41551,14 @@
       <c r="J30">
         <v>1.039200000315905</v>
       </c>
-    </row>
-    <row r="31" spans="1:10">
+      <c r="K30">
+        <v>-0.2275415512271826</v>
+      </c>
+      <c r="L30">
+        <v>-0.2275415512271826</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12">
       <c r="A31" s="1">
         <v>58</v>
       </c>
@@ -41406,8 +41589,14 @@
       <c r="J31">
         <v>1.423899995684624</v>
       </c>
-    </row>
-    <row r="32" spans="1:10">
+      <c r="K31">
+        <v>-0.2626286135430451</v>
+      </c>
+      <c r="L31">
+        <v>-0.2626286135430451</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12">
       <c r="A32" s="1">
         <v>59</v>
       </c>
@@ -41438,8 +41627,14 @@
       <c r="J32">
         <v>3.056400001645089</v>
       </c>
-    </row>
-    <row r="33" spans="1:10">
+      <c r="K32">
+        <v>-0.3346020869518911</v>
+      </c>
+      <c r="L32">
+        <v>-0.3346020869518911</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12">
       <c r="A33" s="1">
         <v>60</v>
       </c>
@@ -41469,6 +41664,12 @@
       </c>
       <c r="J33">
         <v>4.46700000166893</v>
+      </c>
+      <c r="K33">
+        <v>-0.2923523941405345</v>
+      </c>
+      <c r="L33">
+        <v>-0.2923523941405345</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Clean python code, update main.xlsx
</commit_message>
<xml_diff>
--- a/data/main.xlsx
+++ b/data/main.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3113" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3112" uniqueCount="111">
   <si>
     <t>ISO2</t>
   </si>
@@ -349,9 +349,6 @@
   </si>
   <si>
     <t>ev sales share change</t>
-  </si>
-  <si>
-    <t>Emission change since 1990</t>
   </si>
 </sst>
 </file>
@@ -40433,13 +40430,13 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L33"/>
+  <dimension ref="A1:K33"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:11">
       <c r="B1" s="1" t="s">
         <v>2</v>
       </c>
@@ -40468,13 +40465,10 @@
         <v>10</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="L1" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:12">
+    <row r="2" spans="1:11">
       <c r="A2" s="1">
         <v>29</v>
       </c>
@@ -40505,11 +40499,8 @@
       <c r="K2">
         <v>0</v>
       </c>
-      <c r="L2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12">
+    </row>
+    <row r="3" spans="1:11">
       <c r="A3" s="1">
         <v>30</v>
       </c>
@@ -40543,11 +40534,8 @@
       <c r="K3">
         <v>-0.01202191061694069</v>
       </c>
-      <c r="L3">
-        <v>-0.01202191061694069</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12">
+    </row>
+    <row r="4" spans="1:11">
       <c r="A4" s="1">
         <v>31</v>
       </c>
@@ -40581,11 +40569,8 @@
       <c r="K4">
         <v>-0.04351763000623127</v>
       </c>
-      <c r="L4">
-        <v>-0.04351763000623127</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12">
+    </row>
+    <row r="5" spans="1:11">
       <c r="A5" s="1">
         <v>32</v>
       </c>
@@ -40619,11 +40604,8 @@
       <c r="K5">
         <v>-0.061601803895558</v>
       </c>
-      <c r="L5">
-        <v>-0.061601803895558</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12">
+    </row>
+    <row r="6" spans="1:11">
       <c r="A6" s="1">
         <v>33</v>
       </c>
@@ -40657,11 +40639,8 @@
       <c r="K6">
         <v>-0.06669553566309869</v>
       </c>
-      <c r="L6">
-        <v>-0.06669553566309869</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12">
+    </row>
+    <row r="7" spans="1:11">
       <c r="A7" s="1">
         <v>34</v>
       </c>
@@ -40695,11 +40674,8 @@
       <c r="K7">
         <v>-0.05751285579002759</v>
       </c>
-      <c r="L7">
-        <v>-0.05751285579002759</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12">
+    </row>
+    <row r="8" spans="1:11">
       <c r="A8" s="1">
         <v>35</v>
       </c>
@@ -40730,11 +40706,8 @@
       <c r="K8">
         <v>-0.03369104134656577</v>
       </c>
-      <c r="L8">
-        <v>-0.03369104134656577</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12">
+    </row>
+    <row r="9" spans="1:11">
       <c r="A9" s="1">
         <v>36</v>
       </c>
@@ -40765,11 +40738,8 @@
       <c r="K9">
         <v>-0.05364898870356756</v>
       </c>
-      <c r="L9">
-        <v>-0.05364898870356756</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12">
+    </row>
+    <row r="10" spans="1:11">
       <c r="A10" s="1">
         <v>37</v>
       </c>
@@ -40800,11 +40770,8 @@
       <c r="K10">
         <v>-0.05397081384077276</v>
       </c>
-      <c r="L10">
-        <v>-0.05397081384077276</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12">
+    </row>
+    <row r="11" spans="1:11">
       <c r="A11" s="1">
         <v>38</v>
       </c>
@@ -40838,11 +40805,8 @@
       <c r="K11">
         <v>-0.06743642905450249</v>
       </c>
-      <c r="L11">
-        <v>-0.06743642905450249</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12">
+    </row>
+    <row r="12" spans="1:11">
       <c r="A12" s="1">
         <v>39</v>
       </c>
@@ -40876,11 +40840,8 @@
       <c r="K12">
         <v>-0.06347046317449073</v>
       </c>
-      <c r="L12">
-        <v>-0.06347046317449073</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12">
+    </row>
+    <row r="13" spans="1:11">
       <c r="A13" s="1">
         <v>40</v>
       </c>
@@ -40914,11 +40875,8 @@
       <c r="K13">
         <v>-0.04824994195643079</v>
       </c>
-      <c r="L13">
-        <v>-0.04824994195643079</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12">
+    </row>
+    <row r="14" spans="1:11">
       <c r="A14" s="1">
         <v>41</v>
       </c>
@@ -40952,11 +40910,8 @@
       <c r="K14">
         <v>-0.05235420932691991</v>
       </c>
-      <c r="L14">
-        <v>-0.05235420932691991</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12">
+    </row>
+    <row r="15" spans="1:11">
       <c r="A15" s="1">
         <v>42</v>
       </c>
@@ -40990,11 +40945,8 @@
       <c r="K15">
         <v>-0.03101825529906309</v>
       </c>
-      <c r="L15">
-        <v>-0.03101825529906309</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12">
+    </row>
+    <row r="16" spans="1:11">
       <c r="A16" s="1">
         <v>43</v>
       </c>
@@ -41028,11 +40980,8 @@
       <c r="K16">
         <v>-0.02796066617184709</v>
       </c>
-      <c r="L16">
-        <v>-0.02796066617184709</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12">
+    </row>
+    <row r="17" spans="1:11">
       <c r="A17" s="1">
         <v>44</v>
       </c>
@@ -41066,11 +41015,8 @@
       <c r="K17">
         <v>-0.03309562249927574</v>
       </c>
-      <c r="L17">
-        <v>-0.03309562249927574</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12">
+    </row>
+    <row r="18" spans="1:11">
       <c r="A18" s="1">
         <v>45</v>
       </c>
@@ -41101,11 +41047,8 @@
       <c r="K18">
         <v>-0.03141587660430183</v>
       </c>
-      <c r="L18">
-        <v>-0.03141587660430183</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12">
+    </row>
+    <row r="19" spans="1:11">
       <c r="A19" s="1">
         <v>46</v>
       </c>
@@ -41136,11 +41079,8 @@
       <c r="K19">
         <v>-0.04093695694979146</v>
       </c>
-      <c r="L19">
-        <v>-0.04093695694979146</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12">
+    </row>
+    <row r="20" spans="1:11">
       <c r="A20" s="1">
         <v>47</v>
       </c>
@@ -41174,11 +41114,8 @@
       <c r="K20">
         <v>-0.06233409527205656</v>
       </c>
-      <c r="L20">
-        <v>-0.06233409527205656</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12">
+    </row>
+    <row r="21" spans="1:11">
       <c r="A21" s="1">
         <v>48</v>
       </c>
@@ -41212,11 +41149,8 @@
       <c r="K21">
         <v>-0.138952652113448</v>
       </c>
-      <c r="L21">
-        <v>-0.138952652113448</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12">
+    </row>
+    <row r="22" spans="1:11">
       <c r="A22" s="1">
         <v>49</v>
       </c>
@@ -41250,11 +41184,8 @@
       <c r="K22">
         <v>-0.1121153920739042</v>
       </c>
-      <c r="L22">
-        <v>-0.1121153920739042</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12">
+    </row>
+    <row r="23" spans="1:11">
       <c r="A23" s="1">
         <v>50</v>
       </c>
@@ -41288,11 +41219,8 @@
       <c r="K23">
         <v>-0.1444294180427219</v>
       </c>
-      <c r="L23">
-        <v>-0.1444294180427219</v>
-      </c>
-    </row>
-    <row r="24" spans="1:12">
+    </row>
+    <row r="24" spans="1:11">
       <c r="A24" s="1">
         <v>51</v>
       </c>
@@ -41326,11 +41254,8 @@
       <c r="K24">
         <v>-0.1563513303875175</v>
       </c>
-      <c r="L24">
-        <v>-0.1563513303875175</v>
-      </c>
-    </row>
-    <row r="25" spans="1:12">
+    </row>
+    <row r="25" spans="1:11">
       <c r="A25" s="1">
         <v>52</v>
       </c>
@@ -41364,11 +41289,8 @@
       <c r="K25">
         <v>-0.1765019482381661</v>
       </c>
-      <c r="L25">
-        <v>-0.1765019482381661</v>
-      </c>
-    </row>
-    <row r="26" spans="1:12">
+    </row>
+    <row r="26" spans="1:11">
       <c r="A26" s="1">
         <v>53</v>
       </c>
@@ -41402,11 +41324,8 @@
       <c r="K26">
         <v>-0.2159172358664213</v>
       </c>
-      <c r="L26">
-        <v>-0.2159172358664213</v>
-      </c>
-    </row>
-    <row r="27" spans="1:12">
+    </row>
+    <row r="27" spans="1:11">
       <c r="A27" s="1">
         <v>54</v>
       </c>
@@ -41440,11 +41359,8 @@
       <c r="K27">
         <v>-0.2079325709182091</v>
       </c>
-      <c r="L27">
-        <v>-0.2079325709182091</v>
-      </c>
-    </row>
-    <row r="28" spans="1:12">
+    </row>
+    <row r="28" spans="1:11">
       <c r="A28" s="1">
         <v>55</v>
       </c>
@@ -41478,11 +41394,8 @@
       <c r="K28">
         <v>-0.2115464138571911</v>
       </c>
-      <c r="L28">
-        <v>-0.2115464138571911</v>
-      </c>
-    </row>
-    <row r="29" spans="1:12">
+    </row>
+    <row r="29" spans="1:11">
       <c r="A29" s="1">
         <v>56</v>
       </c>
@@ -41516,11 +41429,8 @@
       <c r="K29">
         <v>-0.209345677212742</v>
       </c>
-      <c r="L29">
-        <v>-0.209345677212742</v>
-      </c>
-    </row>
-    <row r="30" spans="1:12">
+    </row>
+    <row r="30" spans="1:11">
       <c r="A30" s="1">
         <v>57</v>
       </c>
@@ -41554,11 +41464,8 @@
       <c r="K30">
         <v>-0.2275415512271826</v>
       </c>
-      <c r="L30">
-        <v>-0.2275415512271826</v>
-      </c>
-    </row>
-    <row r="31" spans="1:12">
+    </row>
+    <row r="31" spans="1:11">
       <c r="A31" s="1">
         <v>58</v>
       </c>
@@ -41592,11 +41499,8 @@
       <c r="K31">
         <v>-0.2626286135430451</v>
       </c>
-      <c r="L31">
-        <v>-0.2626286135430451</v>
-      </c>
-    </row>
-    <row r="32" spans="1:12">
+    </row>
+    <row r="32" spans="1:11">
       <c r="A32" s="1">
         <v>59</v>
       </c>
@@ -41630,11 +41534,8 @@
       <c r="K32">
         <v>-0.3346020869518911</v>
       </c>
-      <c r="L32">
-        <v>-0.3346020869518911</v>
-      </c>
-    </row>
-    <row r="33" spans="1:12">
+    </row>
+    <row r="33" spans="1:11">
       <c r="A33" s="1">
         <v>60</v>
       </c>
@@ -41666,9 +41567,6 @@
         <v>4.46700000166893</v>
       </c>
       <c r="K33">
-        <v>-0.2923523941405345</v>
-      </c>
-      <c r="L33">
         <v>-0.2923523941405345</v>
       </c>
     </row>

</xml_diff>